<commit_message>
docs: update README.md; sample_data: update template workbook
</commit_message>
<xml_diff>
--- a/sample_data/Crypto_Investment_Tracker_template.xlsx
+++ b/sample_data/Crypto_Investment_Tracker_template.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4312d1791fd26735/Documents/Crypto/crypto_tracker_repo/sample_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_04E820EBA9D6995C849B68F3E61AC271382B988E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{087F9724-FB58-4047-A79B-D75FB67C74FB}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-24120" yWindow="450" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -34,8 +40,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,13 +104,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -142,7 +156,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -176,6 +190,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -210,9 +225,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -385,14 +401,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Add runtime dependencies and sample data
</commit_message>
<xml_diff>
--- a/sample_data/Crypto_Investment_Tracker_template.xlsx
+++ b/sample_data/Crypto_Investment_Tracker_template.xlsx
@@ -8,39 +8,97 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4312d1791fd26735/Documents/Crypto/crypto_tracker_repo/sample_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_04E820EBA9D6995C849B68F3E61AC271382B988E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{087F9724-FB58-4047-A79B-D75FB67C74FB}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_3793E131EF34636793322177C552A3D39D54C736" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95155058-705F-4956-8D8A-14B2ED576E75}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="450" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Purchases" sheetId="1" r:id="rId1"/>
+    <sheet name="Transactions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Date of Purchase</t>
-  </si>
-  <si>
-    <t>Coin Type</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Coin</t>
   </si>
   <si>
     <t>Quantity</t>
   </si>
   <si>
-    <t>Cost per Coin (USD)</t>
+    <t>CostPerCoinUSD</t>
+  </si>
+  <si>
+    <t>FeesUSD</t>
+  </si>
+  <si>
+    <t>Exchange</t>
+  </si>
+  <si>
+    <t>TxID</t>
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>TotalCostUSD</t>
+  </si>
+  <si>
+    <t>BTC</t>
+  </si>
+  <si>
+    <t>ETH</t>
+  </si>
+  <si>
+    <t>XRP</t>
+  </si>
+  <si>
+    <t>Coinbase</t>
+  </si>
+  <si>
+    <t>Kraken</t>
+  </si>
+  <si>
+    <t>Uphold</t>
+  </si>
+  <si>
+    <t>demo-btc-001</t>
+  </si>
+  <si>
+    <t>demo-btc-002</t>
+  </si>
+  <si>
+    <t>demo-eth-001</t>
+  </si>
+  <si>
+    <t>demo-xrp-001</t>
+  </si>
+  <si>
+    <t>Initial DCA buy</t>
+  </si>
+  <si>
+    <t>Dip buy</t>
+  </si>
+  <si>
+    <t>Split into staking later</t>
+  </si>
+  <si>
+    <t>Test transfer after buy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -93,11 +151,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,20 +461,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -430,6 +487,292 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>45870</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>0.15</v>
+      </c>
+      <c r="D2">
+        <v>62000</v>
+      </c>
+      <c r="E2">
+        <v>3.5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2">
+        <v>9303.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>45884</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D3">
+        <v>58500</v>
+      </c>
+      <c r="E3">
+        <v>2.25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>4389.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>45902</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>1.8</v>
+      </c>
+      <c r="D4">
+        <v>2650</v>
+      </c>
+      <c r="E4">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4">
+        <v>4774.1000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>45910</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>1200</v>
+      </c>
+      <c r="D5">
+        <v>0.78</v>
+      </c>
+      <c r="E5">
+        <v>1.2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5">
+        <v>937.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>45870</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>0.15</v>
+      </c>
+      <c r="D2">
+        <v>62000</v>
+      </c>
+      <c r="E2">
+        <v>3.5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2">
+        <v>9303.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>45884</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D3">
+        <v>58500</v>
+      </c>
+      <c r="E3">
+        <v>2.25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>4389.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>45902</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>1.8</v>
+      </c>
+      <c r="D4">
+        <v>2650</v>
+      </c>
+      <c r="E4">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4">
+        <v>4774.1000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>45910</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>1200</v>
+      </c>
+      <c r="D5">
+        <v>0.78</v>
+      </c>
+      <c r="E5">
+        <v>1.2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5">
+        <v>937.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>